<commit_message>
excel de informacion del circuito
</commit_message>
<xml_diff>
--- a/Ej8/Others/datos_componentes.xlsx
+++ b/Ej8/Others/datos_componentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalo\Desktop\ITBA\ELECTRO 3\TP 2\git\tp2-grupo-2\Ej8\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A677A3E-7845-4286-AA98-1130B9E86D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD5F34B-2077-4E33-9FDB-BF8B2779611F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A65B092E-94F7-4940-B86C-3D1594170EDB}"/>
   </bookViews>
@@ -429,9 +429,6 @@
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -483,6 +480,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -802,54 +802,54 @@
   <dimension ref="C6:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="6" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="7"/>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="22">
+      <c r="C8" s="21">
         <v>555</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>555</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
@@ -858,22 +858,22 @@
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="9">
         <v>80</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <v>80</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="9">
         <v>90</v>
       </c>
-      <c r="J9" s="16"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
@@ -882,20 +882,20 @@
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>32</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="10">
+      <c r="H10" s="10"/>
+      <c r="I10" s="9">
         <v>32</v>
       </c>
-      <c r="J10" s="16"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
@@ -904,18 +904,18 @@
       <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="10">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9">
         <v>80</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="16">
         <v>100</v>
       </c>
     </row>
@@ -926,18 +926,18 @@
       <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="10">
+      <c r="G12" s="10"/>
+      <c r="H12" s="9">
         <v>300</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="16"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="15"/>
     </row>
     <row r="13" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
@@ -946,18 +946,18 @@
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="20">
+      <c r="G13" s="18"/>
+      <c r="H13" s="19">
         <v>20</v>
       </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="21"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>